<commit_message>
Updated the student accommodation file.
</commit_message>
<xml_diff>
--- a/irp-webapp/src/main/resources/irp-package/IRPStudentsDesignatedSupportsAndAccommodations.xlsx
+++ b/irp-webapp/src/main/resources/irp-package/IRPStudentsDesignatedSupportsAndAccommodations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="8440" windowWidth="38340" windowHeight="15120"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="38160" windowHeight="15820"/>
   </bookViews>
   <sheets>
     <sheet name="DESIGNATEDSUPPORTSANDACCOMMODAT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="74">
   <si>
     <t>StudentIdentifier</t>
   </si>
@@ -72,55 +72,175 @@
     <t>Other</t>
   </si>
   <si>
-    <t>39990004</t>
-  </si>
-  <si>
     <t>CA</t>
   </si>
   <si>
     <t>ELA</t>
   </si>
   <si>
-    <t>TDS_ASL0</t>
-  </si>
-  <si>
     <t>TDS_CC0</t>
   </si>
   <si>
     <t>TDS_ClosedCap0</t>
   </si>
   <si>
-    <t>ENU</t>
-  </si>
-  <si>
     <t>TDS_Masking0</t>
   </si>
   <si>
-    <t>TDS_PM0</t>
-  </si>
-  <si>
-    <t>TDS_PoD0</t>
-  </si>
-  <si>
     <t>TDS_PS_L1</t>
   </si>
   <si>
     <t>TDS_SLM0</t>
   </si>
   <si>
-    <t>TDS_TTS0</t>
-  </si>
-  <si>
     <t>TDS_WL_Glossary</t>
   </si>
   <si>
-    <t>NEDS_BD</t>
-  </si>
-  <si>
-    <t>NEA_Calc</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>TDS_CCMagenta</t>
+  </si>
+  <si>
+    <t>TDS_Masking1</t>
+  </si>
+  <si>
+    <t>TDS_PoD_Stim</t>
+  </si>
+  <si>
+    <t>TDS_PS_L3</t>
+  </si>
+  <si>
+    <t>TDS_SLM1</t>
+  </si>
+  <si>
+    <t>NEDS_CC;NEDS_Mag;NEDS_NoiseBuf;NEDS_RA_Items;</t>
+  </si>
+  <si>
+    <t>NEA_RA_Stimuli;</t>
+  </si>
+  <si>
+    <t>TDS_CCInvert</t>
+  </si>
+  <si>
+    <t>TDS_TTS_Item</t>
+  </si>
+  <si>
+    <t>NEDS_BD;NEDS_CC;NEDS_NoiseBuf;NEDS_TransDirs;</t>
+  </si>
+  <si>
+    <t>TDS_PS_L0</t>
+  </si>
+  <si>
+    <t>TDS_TTS_Stim&amp;TDS_TTS_Item</t>
+  </si>
+  <si>
+    <t>NEDS_CC;NEDS_Mag;NEDS_RA_Items;</t>
+  </si>
+  <si>
+    <t>TDS_ASL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TDS_PoD0</t>
+  </si>
+  <si>
+    <t>NEDS_CC;NEDS_CO;NEDS_Mag;NEDS_NoiseBuf;NEDS_SS;</t>
+  </si>
+  <si>
+    <t>NEA_RA_Stimuli;NEA_STT;</t>
+  </si>
+  <si>
+    <t>TDS_ClosedCap1</t>
+  </si>
+  <si>
+    <t>TDS_TTS_Stim</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>TDS_WL_KoreanGloss</t>
+  </si>
+  <si>
+    <t>NEDS_CO;</t>
+  </si>
+  <si>
+    <t>NEA_Calc;</t>
+  </si>
+  <si>
+    <t>TDS_CCMedGrayLtGray</t>
+  </si>
+  <si>
+    <t>NEDS_CO;NEDS_Mag;NEDS_RA_Items;NEDS_SS;</t>
+  </si>
+  <si>
+    <t>NEA_Abacus;NEA_STT;</t>
+  </si>
+  <si>
+    <t>NEDS_BD;NEDS_Mag;NEDS_RA_Items;NEDS_SS;</t>
+  </si>
+  <si>
+    <t>NEDS_NoiseBuf;NEDS_RA_Items;NEDS_TransDirs;</t>
+  </si>
+  <si>
+    <t>NEDS_SS;</t>
+  </si>
+  <si>
+    <t>NEDS_RA_Items;</t>
+  </si>
+  <si>
+    <t>NEA_AR;</t>
+  </si>
+  <si>
+    <t>TDS_CCYellowB</t>
+  </si>
+  <si>
+    <t>TDS_PS_L2</t>
+  </si>
+  <si>
+    <t>NEDS_CC;</t>
+  </si>
+  <si>
+    <t>NEA_AR;NEA_RA_Stimuli;NEA_STT;</t>
+  </si>
+  <si>
+    <t>NEA_AR;NEA_Calc;</t>
+  </si>
+  <si>
+    <t>NEDS_CC;NEDS_Mag;</t>
+  </si>
+  <si>
+    <t>NEDS_CO;NEDS_RA_Items;</t>
+  </si>
+  <si>
+    <t>NEA_Abacus;</t>
+  </si>
+  <si>
+    <t>NEDS_CC;NEDS_SS;</t>
+  </si>
+  <si>
+    <t>NEA_Calc;NEA_STT;</t>
+  </si>
+  <si>
+    <t>TDS_WL_CantoneseGloss</t>
+  </si>
+  <si>
+    <t>TDS_WL_ArabicGloss</t>
+  </si>
+  <si>
+    <t>NEDS_BD;</t>
+  </si>
+  <si>
+    <t>NEA_STT;</t>
+  </si>
+  <si>
+    <t>NEDS_BD;NEDS_CC;NEDS_CO;NEDS_SS;NEDS_TUkrainian;</t>
+  </si>
+  <si>
+    <t>TDS_WL_ESNGlossary&amp;TDS_WL_Glossary</t>
+  </si>
+  <si>
+    <t>NEDS_CC;NEDS_CO;NEDS_Mag;NEDS_RA_Items;</t>
+  </si>
+  <si>
+    <t>NEA_Abacus;NEA_AR;NEA_RA_Stimuli;</t>
   </si>
 </sst>
 </file>
@@ -490,9 +610,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -503,13 +625,13 @@
     <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27.5" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25.5" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -569,57 +691,1162 @@
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2">
+        <v>39990001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2"/>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3">
+        <v>39990002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4">
+        <v>39990003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4"/>
+      <c r="O4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4"/>
+      <c r="Q4"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5">
+        <v>39990004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G5"/>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6">
+        <v>39990005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7">
+        <v>39990006</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8">
+        <v>39990007</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" t="s">
+        <v>46</v>
+      </c>
+      <c r="P8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9">
+        <v>39990008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10">
+        <v>39990009</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10" t="s">
+        <v>49</v>
+      </c>
+      <c r="P10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11">
+        <v>39990010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" t="s">
+        <v>51</v>
+      </c>
+      <c r="P11"/>
+      <c r="Q11"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12">
+        <v>39990011</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12" t="s">
+        <v>52</v>
+      </c>
+      <c r="P12" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q12"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13">
+        <v>39990012</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P13"/>
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14">
+        <v>79990001</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15">
+        <v>79990002</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16">
+        <v>79990003</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16"/>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" t="s">
+        <v>43</v>
+      </c>
+      <c r="N16"/>
+      <c r="O16" t="s">
+        <v>58</v>
+      </c>
+      <c r="P16" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17">
+        <v>79990004</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18">
+        <v>79990005</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q18"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19">
+        <v>79990006</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19" t="s">
+        <v>54</v>
+      </c>
+      <c r="P19"/>
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20">
+        <v>79990007</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20" t="s">
+        <v>36</v>
+      </c>
+      <c r="N20"/>
+      <c r="O20" t="s">
+        <v>58</v>
+      </c>
+      <c r="P20"/>
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21">
+        <v>79990008</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21"/>
+      <c r="O21" t="s">
+        <v>61</v>
+      </c>
+      <c r="P21"/>
+      <c r="Q21"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22">
+        <v>79990009</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23">
+        <v>79990010</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23"/>
+      <c r="O23" t="s">
+        <v>58</v>
+      </c>
+      <c r="P23"/>
+      <c r="Q23"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24">
+        <v>79990011</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N24"/>
+      <c r="O24" t="s">
+        <v>62</v>
+      </c>
+      <c r="P24" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q24"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25">
+        <v>79990012</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25" t="s">
+        <v>43</v>
+      </c>
+      <c r="N25"/>
+      <c r="O25" t="s">
+        <v>64</v>
+      </c>
+      <c r="P25"/>
+      <c r="Q25"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26">
+        <v>119990001</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26" t="s">
+        <v>54</v>
+      </c>
+      <c r="P26" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q26"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27">
+        <v>119990002</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27"/>
+      <c r="H27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27"/>
+      <c r="J27" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" t="s">
+        <v>28</v>
+      </c>
+      <c r="L27"/>
+      <c r="M27" t="s">
+        <v>33</v>
+      </c>
+      <c r="N27" t="s">
+        <v>66</v>
+      </c>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28">
+        <v>119990003</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28" t="s">
+        <v>67</v>
+      </c>
+      <c r="O28"/>
+      <c r="P28" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q28"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29">
+        <v>119990004</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29" t="s">
+        <v>68</v>
+      </c>
+      <c r="P29" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q29"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30">
+        <v>119990005</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31">
+        <v>119990006</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32">
+        <v>119990007</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32" t="s">
+        <v>43</v>
+      </c>
+      <c r="N32"/>
+      <c r="O32" t="s">
+        <v>70</v>
+      </c>
+      <c r="P32" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q32"/>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33">
+        <v>119990008</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33" t="s">
+        <v>71</v>
+      </c>
+      <c r="O33"/>
+      <c r="P33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q33"/>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34">
+        <v>119990009</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" t="s">
+        <v>57</v>
+      </c>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35">
+        <v>119990010</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35" t="s">
+        <v>46</v>
+      </c>
+      <c r="P35" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q35"/>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36">
+        <v>119990011</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36" t="s">
         <v>33</v>
       </c>
+      <c r="N36"/>
+      <c r="O36" t="s">
+        <v>72</v>
+      </c>
+      <c r="P36" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q36"/>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37">
+        <v>119990012</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37" t="s">
+        <v>43</v>
+      </c>
+      <c r="N37"/>
+      <c r="O37" t="s">
+        <v>46</v>
+      </c>
+      <c r="P37" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>